<commit_message>
Update matrix and list
</commit_message>
<xml_diff>
--- a/Table Relations Matrix.xlsx
+++ b/Table Relations Matrix.xlsx
@@ -935,8 +935,8 @@
       <c r="T11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="U11" s="5" t="s">
-        <v>23</v>
+      <c r="U11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="V11" s="5" t="s">
         <v>23</v>
@@ -1583,8 +1583,8 @@
       <c r="J21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K21" s="5" t="s">
-        <v>23</v>
+      <c r="K21" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>21</v>
@@ -1652,7 +1652,7 @@
         <v>21</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>21</v>

</xml_diff>